<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T05:39:55.892Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -399,13 +399,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Order ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Flat No</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Items</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Total</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Payment</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Collection Date</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Collection Time</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Notes</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Cancel Reason</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Feedback</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-01-19 05:39</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Prajakta Patil</v>
+      </c>
+      <c r="D2" t="str">
+        <v>A 804</v>
+      </c>
+      <c r="E2" t="str">
+        <v>779868817</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+      </c>
+      <c r="G2">
+        <v>105</v>
+      </c>
+      <c r="H2" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I2" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J2" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K2" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -445,10 +534,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -463,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -478,13 +567,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Item</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Quantity Ordered</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Revenue</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Wheat Chapati</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1 Plate Bhaji</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T05:41:03.627Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,10 +450,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C2" t="str">
         <v>Prajakta Patil</v>
@@ -477,13 +477,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
         <v>08:00</v>
       </c>
       <c r="L2" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -492,9 +492,53 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-19 05:39</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Prajakta Patil</v>
+      </c>
+      <c r="D3" t="str">
+        <v>A 804</v>
+      </c>
+      <c r="E3" t="str">
+        <v>779868817</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+      </c>
+      <c r="G3">
+        <v>105</v>
+      </c>
+      <c r="H3" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J3" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K3" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -534,10 +578,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -552,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -588,10 +632,10 @@
         <v>Wheat Chapati</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3">
@@ -599,10 +643,10 @@
         <v>1 Plate Bhaji</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T05:42:02.387Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,10 +450,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C2" t="str">
         <v>Prajakta Patil</v>
@@ -465,10 +465,10 @@
         <v>779868817</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,7 +477,7 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K2" t="str">
         <v>08:00</v>
@@ -494,10 +494,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C3" t="str">
         <v>Prajakta Patil</v>
@@ -521,13 +521,13 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K3" t="str">
         <v>08:00</v>
       </c>
       <c r="L3" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -536,9 +536,53 @@
         <v/>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-19 05:39</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Prajakta Patil</v>
+      </c>
+      <c r="D4" t="str">
+        <v>A 804</v>
+      </c>
+      <c r="E4" t="str">
+        <v>779868817</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+      </c>
+      <c r="G4">
+        <v>105</v>
+      </c>
+      <c r="H4" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I4" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J4" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K4" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L4" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -578,10 +622,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -596,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>210</v>
+        <v>285</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -632,10 +676,10 @@
         <v>Wheat Chapati</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3">
@@ -643,10 +687,10 @@
         <v>1 Plate Bhaji</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T08:37:38.781Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C2" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D2" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E2" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x3</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,7 +477,7 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K2" t="str">
         <v>08:00</v>
@@ -494,10 +494,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C3" t="str">
         <v>Prajakta Patil</v>
@@ -509,10 +509,10 @@
         <v>779868817</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G3">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,7 +521,7 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K3" t="str">
         <v>08:00</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C4" t="str">
         <v>Prajakta Patil</v>
@@ -565,24 +565,68 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K4" t="str">
         <v>08:00</v>
       </c>
       <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-19 05:39</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Prajakta Patil</v>
+      </c>
+      <c r="D5" t="str">
+        <v>A 804</v>
+      </c>
+      <c r="E5" t="str">
+        <v>779868817</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+      </c>
+      <c r="G5">
+        <v>105</v>
+      </c>
+      <c r="H5" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J5" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K5" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L5" t="str">
         <v>Less Spicy</v>
       </c>
-      <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -622,10 +666,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -640,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>285</v>
+        <v>375</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -655,7 +699,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -684,7 +728,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1 Plate Bhaji</v>
+        <v>Pohe</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -693,9 +737,20 @@
         <v>90</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1 Plate Bhaji</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T09:13:42.591Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -465,10 +465,10 @@
         <v>9967195227</v>
       </c>
       <c r="F2" t="str">
-        <v>Pohe x3</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G2">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>375</v>
+        <v>405</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -699,7 +699,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -720,15 +720,15 @@
         <v>Wheat Chapati</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>195</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Pohe</v>
+        <v>1 Plate Bhaji</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -739,18 +739,29 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>1 Plate Bhaji</v>
+        <v>Pohe</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>90</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Upma</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T09:18:12.777Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,22 +450,22 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C2" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D2" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E2" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F2" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G2">
         <v>120</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K2" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C3" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D3" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E3" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G3">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,7 +521,7 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K3" t="str">
         <v>08:00</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C4" t="str">
         <v>Prajakta Patil</v>
@@ -553,10 +553,10 @@
         <v>779868817</v>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G4">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -565,7 +565,7 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K4" t="str">
         <v>08:00</v>
@@ -582,10 +582,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C5" t="str">
         <v>Prajakta Patil</v>
@@ -609,24 +609,68 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K5" t="str">
         <v>08:00</v>
       </c>
       <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-19 05:39</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Prajakta Patil</v>
+      </c>
+      <c r="D6" t="str">
+        <v>A 804</v>
+      </c>
+      <c r="E6" t="str">
+        <v>779868817</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+      </c>
+      <c r="G6">
+        <v>105</v>
+      </c>
+      <c r="H6" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I6" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J6" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K6" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L6" t="str">
         <v>Less Spicy</v>
       </c>
-      <c r="M5" t="str">
-        <v/>
-      </c>
-      <c r="N5" t="str">
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -666,10 +710,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -684,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>405</v>
+        <v>525</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -699,7 +743,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -728,40 +772,51 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1 Plate Bhaji</v>
+        <v>Til Poli</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Pohe</v>
+        <v>1 Plate Bhaji</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>Pohe</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
         <v>Upma</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T09:18:42.609Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -471,7 +471,7 @@
         <v>120</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -713,7 +713,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T09:18:45.317Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -474,7 +474,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-18</v>
@@ -518,7 +518,7 @@
         <v>NEW</v>
       </c>
       <c r="I3" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J3" t="str">
         <v>2026-01-20</v>
@@ -731,7 +731,7 @@
         <v>525</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T09:18:47.181Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -515,7 +515,7 @@
         <v>120</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
         <v>PAID</v>
@@ -713,7 +713,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-19.xlsx - 2026-01-19T09:19:18.058Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-19.xlsx
@@ -515,7 +515,7 @@
         <v>120</v>
       </c>
       <c r="H3" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PAID</v>
@@ -713,7 +713,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>